<commit_message>
Update state dropdown selector
</commit_message>
<xml_diff>
--- a/InputData/indst/CoNEPPpCAPS/Cal of Nutritionally Equiv Plant Products per Cal Animal Prd Shifted.xlsx
+++ b/InputData/indst/CoNEPPpCAPS/Cal of Nutritionally Equiv Plant Products per Cal Animal Prd Shifted.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10411"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/users/nathaniyer/library/containers/com.microsoft.excel/data/state-eps-data-repository/or/indst/conepppcaps/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-oregon\InputData\indst\CoNEPPpCAPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8EFCC28-1BF1-D646-BA1F-C65EC21BFE08}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4700" yWindow="2100" windowWidth="24100" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4703" yWindow="2100" windowWidth="24098" windowHeight="14160"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -21,7 +20,7 @@
     <sheet name="Calculations" sheetId="2" r:id="rId6"/>
     <sheet name="CoNEPPpCAPS" sheetId="3" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -348,7 +347,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
@@ -477,7 +476,7 @@
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -803,30 +802,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="1" max="1" width="12.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="C1" s="19">
         <v>44307</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
@@ -834,12 +833,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="K4" s="16" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -855,7 +854,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -863,7 +862,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B7" s="2">
         <v>2018</v>
       </c>
@@ -871,7 +870,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
         <v>2</v>
       </c>
@@ -879,7 +878,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B9" s="3" t="s">
         <v>4</v>
       </c>
@@ -887,7 +886,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
         <v>1</v>
       </c>
@@ -895,12 +894,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="K11" s="16" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B12" s="13" t="s">
         <v>90</v>
       </c>
@@ -913,7 +912,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
         <v>19</v>
       </c>
@@ -921,7 +920,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B14">
         <v>2019</v>
       </c>
@@ -929,7 +928,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B15" t="s">
         <v>93</v>
       </c>
@@ -937,7 +936,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B16" s="3" t="s">
         <v>23</v>
       </c>
@@ -945,7 +944,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B17" t="s">
         <v>94</v>
       </c>
@@ -953,12 +952,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.45">
       <c r="K18" s="16" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B19" s="13" t="s">
         <v>95</v>
       </c>
@@ -971,7 +970,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
         <v>19</v>
       </c>
@@ -979,7 +978,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B21" s="2">
         <v>2020</v>
       </c>
@@ -987,7 +986,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B22" t="s">
         <v>96</v>
       </c>
@@ -995,7 +994,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B23" s="3" t="s">
         <v>26</v>
       </c>
@@ -1003,12 +1002,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.45">
       <c r="K24" s="16" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B25" s="13" t="s">
         <v>97</v>
       </c>
@@ -1021,7 +1020,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B26" t="s">
         <v>19</v>
       </c>
@@ -1029,7 +1028,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B27" s="2">
         <v>2020</v>
       </c>
@@ -1037,7 +1036,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B28" t="s">
         <v>98</v>
       </c>
@@ -1045,7 +1044,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B29" s="3" t="s">
         <v>25</v>
       </c>
@@ -1053,12 +1052,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.45">
       <c r="K30" s="16" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B31" s="13" t="s">
         <v>91</v>
       </c>
@@ -1071,7 +1070,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B32" t="s">
         <v>19</v>
       </c>
@@ -1079,7 +1078,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B33" s="2">
         <v>2017</v>
       </c>
@@ -1087,7 +1086,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B34" t="s">
         <v>99</v>
       </c>
@@ -1095,7 +1094,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B35" s="3" t="s">
         <v>22</v>
       </c>
@@ -1103,12 +1102,12 @@
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
       <c r="K36" s="16" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B37" s="13" t="s">
         <v>92</v>
       </c>
@@ -1121,7 +1120,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B38" t="s">
         <v>19</v>
       </c>
@@ -1129,7 +1128,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B39" s="2">
         <v>2020</v>
       </c>
@@ -1137,7 +1136,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B40" t="s">
         <v>100</v>
       </c>
@@ -1145,7 +1144,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B41" s="3" t="s">
         <v>24</v>
       </c>
@@ -1153,12 +1152,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
       <c r="K42" s="16" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>5</v>
       </c>
@@ -1166,7 +1165,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>15</v>
       </c>
@@ -1174,7 +1173,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>16</v>
       </c>
@@ -1182,7 +1181,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>89</v>
       </c>
@@ -1190,45 +1189,45 @@
         <v>70</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
       <c r="K47" s="16" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
       <c r="K48" s="16" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="49" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="11:11" x14ac:dyDescent="0.45">
       <c r="K49" s="16" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="50" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="11:11" x14ac:dyDescent="0.45">
       <c r="K50" s="16" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="51" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="11:11" x14ac:dyDescent="0.45">
       <c r="K51" s="16" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="52" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="11:11" x14ac:dyDescent="0.45">
       <c r="K52" s="16" t="s">
         <v>76</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
       <formula1>$K$3:$K$52</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B9" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B16" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B9" r:id="rId1"/>
+    <hyperlink ref="B16" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -1236,21 +1235,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="9" style="11"/>
     <col min="3" max="3" width="10.6640625" style="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B1" s="11" t="s">
         <v>80</v>
       </c>
@@ -1264,7 +1263,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A2" s="16" t="s">
         <v>27</v>
       </c>
@@ -1283,7 +1282,7 @@
         <v>30.015999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="16" t="s">
         <v>28</v>
       </c>
@@ -1295,7 +1294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="16" t="s">
         <v>29</v>
       </c>
@@ -1307,7 +1306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="16" t="s">
         <v>30</v>
       </c>
@@ -1319,7 +1318,7 @@
         <v>3868395513.4538274</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="16" t="s">
         <v>31</v>
       </c>
@@ -1331,7 +1330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="16" t="s">
         <v>32</v>
       </c>
@@ -1343,7 +1342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="16" t="s">
         <v>33</v>
       </c>
@@ -1355,7 +1354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="16" t="s">
         <v>34</v>
       </c>
@@ -1367,7 +1366,7 @@
         <v>937792851.74638259</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="16" t="s">
         <v>35</v>
       </c>
@@ -1379,7 +1378,7 @@
         <v>215259743.12779689</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="16" t="s">
         <v>36</v>
       </c>
@@ -1391,7 +1390,7 @@
         <v>4745831905.6198063</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="16" t="s">
         <v>37</v>
       </c>
@@ -1403,7 +1402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="16" t="s">
         <v>38</v>
       </c>
@@ -1415,7 +1414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="16" t="s">
         <v>39</v>
       </c>
@@ -1427,7 +1426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="16" t="s">
         <v>40</v>
       </c>
@@ -1439,7 +1438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="16" t="s">
         <v>41</v>
       </c>
@@ -1451,7 +1450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" s="16" t="s">
         <v>42</v>
       </c>
@@ -1463,7 +1462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" s="16" t="s">
         <v>43</v>
       </c>
@@ -1475,7 +1474,7 @@
         <v>1043852757.5986518</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" s="16" t="s">
         <v>44</v>
       </c>
@@ -1487,7 +1486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" s="16" t="s">
         <v>45</v>
       </c>
@@ -1499,7 +1498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" s="16" t="s">
         <v>46</v>
       </c>
@@ -1511,7 +1510,7 @@
         <v>1029199744.2901148</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" s="16" t="s">
         <v>47</v>
       </c>
@@ -1523,7 +1522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" s="16" t="s">
         <v>48</v>
       </c>
@@ -1535,7 +1534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" s="16" t="s">
         <v>49</v>
       </c>
@@ -1547,7 +1546,7 @@
         <v>222935131.05131638</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" s="16" t="s">
         <v>50</v>
       </c>
@@ -1559,7 +1558,7 @@
         <v>2682896960.5393162</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" s="16" t="s">
         <v>51</v>
       </c>
@@ -1571,7 +1570,7 @@
         <v>1014895612.2508283</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" s="16" t="s">
         <v>52</v>
       </c>
@@ -1583,7 +1582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" s="16" t="s">
         <v>53</v>
       </c>
@@ -1595,7 +1594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A29" s="16" t="s">
         <v>54</v>
       </c>
@@ -1607,7 +1606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30" s="16" t="s">
         <v>55</v>
       </c>
@@ -1619,7 +1618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31" s="16" t="s">
         <v>56</v>
       </c>
@@ -1631,7 +1630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32" s="16" t="s">
         <v>57</v>
       </c>
@@ -1643,7 +1642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A33" s="16" t="s">
         <v>58</v>
       </c>
@@ -1655,7 +1654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34" s="16" t="s">
         <v>59</v>
       </c>
@@ -1667,7 +1666,7 @@
         <v>3196101307.6073699</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35" s="16" t="s">
         <v>60</v>
       </c>
@@ -1679,7 +1678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A36" s="16" t="s">
         <v>61</v>
       </c>
@@ -1691,7 +1690,7 @@
         <v>382722752.3682223</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A37" s="16" t="s">
         <v>62</v>
       </c>
@@ -1703,7 +1702,7 @@
         <v>737186121.92712295</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A38" s="16" t="s">
         <v>63</v>
       </c>
@@ -1715,7 +1714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A39" s="16" t="s">
         <v>64</v>
       </c>
@@ -1727,7 +1726,7 @@
         <v>701949113.7327832</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A40" s="16" t="s">
         <v>65</v>
       </c>
@@ -1739,7 +1738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A41" s="16" t="s">
         <v>66</v>
       </c>
@@ -1751,7 +1750,7 @@
         <v>854759109.66467154</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A42" s="16" t="s">
         <v>67</v>
       </c>
@@ -1763,7 +1762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A43" s="16" t="s">
         <v>68</v>
       </c>
@@ -1775,7 +1774,7 @@
         <v>619962015.45882499</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A44" s="16" t="s">
         <v>69</v>
       </c>
@@ -1787,7 +1786,7 @@
         <v>2354948567.4434829</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A45" s="16" t="s">
         <v>70</v>
       </c>
@@ -1799,7 +1798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A46" s="16" t="s">
         <v>71</v>
       </c>
@@ -1811,7 +1810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A47" s="16" t="s">
         <v>72</v>
       </c>
@@ -1823,7 +1822,7 @@
         <v>981403010.40274334</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A48" s="16" t="s">
         <v>73</v>
       </c>
@@ -1835,7 +1834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A49" s="16" t="s">
         <v>74</v>
       </c>
@@ -1847,7 +1846,7 @@
         <v>263405358.28441918</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A50" s="16" t="s">
         <v>75</v>
       </c>
@@ -1859,7 +1858,7 @@
         <v>204095542.51176852</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A51" s="16" t="s">
         <v>76</v>
       </c>
@@ -1877,25 +1876,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B1" s="17" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="16" t="s">
         <v>27</v>
       </c>
@@ -1903,7 +1902,7 @@
         <v>71538260</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="16" t="s">
         <v>28</v>
       </c>
@@ -1911,7 +1910,7 @@
         <v>3235159</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="16" t="s">
         <v>29</v>
       </c>
@@ -1919,7 +1918,7 @@
         <v>4447022388</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="16" t="s">
         <v>30</v>
       </c>
@@ -1927,7 +1926,7 @@
         <v>106146581</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="16" t="s">
         <v>31</v>
       </c>
@@ -1935,7 +1934,7 @@
         <v>38409628157</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" s="16" t="s">
         <v>32</v>
       </c>
@@ -1943,7 +1942,7 @@
         <v>3236274894</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" s="16" t="s">
         <v>33</v>
       </c>
@@ -1951,7 +1950,7 @@
         <v>354373009</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="16" t="s">
         <v>34</v>
       </c>
@@ -1959,7 +1958,7 @@
         <v>86735436</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" s="16" t="s">
         <v>35</v>
       </c>
@@ -1967,7 +1966,7 @@
         <v>2041382977</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" s="16" t="s">
         <v>36</v>
       </c>
@@ -1975,7 +1974,7 @@
         <v>1471418848</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" s="16" t="s">
         <v>37</v>
       </c>
@@ -1983,7 +1982,7 @@
         <v>19486239</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" s="16" t="s">
         <v>38</v>
       </c>
@@ -1991,7 +1990,7 @@
         <v>13376592795</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" s="16" t="s">
         <v>39</v>
       </c>
@@ -1999,7 +1998,7 @@
         <v>1654260723</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" s="16" t="s">
         <v>40</v>
       </c>
@@ -2007,7 +2006,7 @@
         <v>3109408521</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" s="16" t="s">
         <v>41</v>
       </c>
@@ -2015,7 +2014,7 @@
         <v>4172638418</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" s="16" t="s">
         <v>42</v>
       </c>
@@ -2023,7 +2022,7 @@
         <v>3894112738</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" s="16" t="s">
         <v>43</v>
       </c>
@@ -2031,7 +2030,7 @@
         <v>671143662</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" s="16" t="s">
         <v>44</v>
       </c>
@@ -2039,7 +2038,7 @@
         <v>148943209</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" s="16" t="s">
         <v>45</v>
       </c>
@@ -2047,7 +2046,7 @@
         <v>486333857</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" s="16" t="s">
         <v>46</v>
       </c>
@@ -2055,7 +2054,7 @@
         <v>620678801</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" s="16" t="s">
         <v>47</v>
       </c>
@@ -2063,7 +2062,7 @@
         <v>212751178</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" s="16" t="s">
         <v>48</v>
       </c>
@@ -2071,7 +2070,7 @@
         <v>7100544178</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A24" s="16" t="s">
         <v>49</v>
       </c>
@@ -2079,7 +2078,7 @@
         <v>8255844823</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A25" s="16" t="s">
         <v>50</v>
       </c>
@@ -2087,7 +2086,7 @@
         <v>133723476</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A26" s="16" t="s">
         <v>51</v>
       </c>
@@ -2095,7 +2094,7 @@
         <v>974039139</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A27" s="16" t="s">
         <v>52</v>
       </c>
@@ -2103,7 +2102,7 @@
         <v>305378235</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A28" s="16" t="s">
         <v>53</v>
       </c>
@@ -2111,7 +2110,7 @@
         <v>1313711522</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A29" s="16" t="s">
         <v>54</v>
       </c>
@@ -2119,7 +2118,7 @@
         <v>981291728</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A30" s="16" t="s">
         <v>55</v>
       </c>
@@ -2127,7 +2126,7 @@
         <v>252195925</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A31" s="16" t="s">
         <v>56</v>
       </c>
@@ -2135,7 +2134,7 @@
         <v>87619332</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A32" s="16" t="s">
         <v>57</v>
       </c>
@@ -2143,7 +2142,7 @@
         <v>8096945031</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A33" s="16" t="s">
         <v>58</v>
       </c>
@@ -2151,7 +2150,7 @@
         <v>9842752032</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34" s="16" t="s">
         <v>59</v>
       </c>
@@ -2159,7 +2158,7 @@
         <v>920728230</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A35" s="16" t="s">
         <v>60</v>
       </c>
@@ -2167,7 +2166,7 @@
         <v>242085705</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A36" s="16" t="s">
         <v>61</v>
       </c>
@@ -2175,7 +2174,7 @@
         <v>3940656963</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A37" s="16" t="s">
         <v>62</v>
       </c>
@@ -2183,7 +2182,7 @@
         <v>527182098</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A38" s="16" t="s">
         <v>63</v>
       </c>
@@ -2191,7 +2190,7 @@
         <v>2394966049</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A39" s="16" t="s">
         <v>64</v>
       </c>
@@ -2199,7 +2198,7 @@
         <v>5397908731</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A40" s="16" t="s">
         <v>65</v>
       </c>
@@ -2207,7 +2206,7 @@
         <v>14075892</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A41" s="16" t="s">
         <v>66</v>
       </c>
@@ -2215,7 +2214,7 @@
         <v>126364285</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A42" s="16" t="s">
         <v>67</v>
       </c>
@@ -2223,7 +2222,7 @@
         <v>1855798800</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A43" s="16" t="s">
         <v>68</v>
       </c>
@@ -2231,7 +2230,7 @@
         <v>671035957</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A44" s="16" t="s">
         <v>69</v>
       </c>
@@ -2239,7 +2238,7 @@
         <v>10096430281</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A45" s="16" t="s">
         <v>70</v>
       </c>
@@ -2247,7 +2246,7 @@
         <v>2000043372</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A46" s="16" t="s">
         <v>71</v>
       </c>
@@ -2255,7 +2254,7 @@
         <v>1942653953</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A47" s="16" t="s">
         <v>72</v>
       </c>
@@ -2263,7 +2262,7 @@
         <v>1368686719</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A48" s="16" t="s">
         <v>73</v>
       </c>
@@ -2271,7 +2270,7 @@
         <v>5333821684</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A49" s="16" t="s">
         <v>74</v>
       </c>
@@ -2279,7 +2278,7 @@
         <v>58404272</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A50" s="16" t="s">
         <v>75</v>
       </c>
@@ -2287,7 +2286,7 @@
         <v>23017794952</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A51" s="16" t="s">
         <v>76</v>
       </c>
@@ -2301,20 +2300,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="18" style="17" customWidth="1"/>
     <col min="3" max="3" width="19.6640625" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B1" s="18" t="s">
         <v>77</v>
       </c>
@@ -2322,7 +2321,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="16" t="s">
         <v>27</v>
       </c>
@@ -2333,7 +2332,7 @@
         <v>30388</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="16" t="s">
         <v>28</v>
       </c>
@@ -2344,7 +2343,7 @@
         <v>1191</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="16" t="s">
         <v>29</v>
       </c>
@@ -2355,7 +2354,7 @@
         <v>60218</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" s="16" t="s">
         <v>30</v>
       </c>
@@ -2366,7 +2365,7 @@
         <v>69193</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" s="16" t="s">
         <v>31</v>
       </c>
@@ -2377,7 +2376,7 @@
         <v>35322</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" s="16" t="s">
         <v>32</v>
       </c>
@@ -2388,7 +2387,7 @@
         <v>243273</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" s="16" t="s">
         <v>33</v>
       </c>
@@ -2399,7 +2398,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" s="16" t="s">
         <v>34</v>
       </c>
@@ -2410,7 +2409,7 @@
         <v>6418</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" s="16" t="s">
         <v>35</v>
       </c>
@@ -2421,7 +2420,7 @@
         <v>3221</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" s="16" t="s">
         <v>36</v>
       </c>
@@ -2432,7 +2431,7 @@
         <v>68391</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" s="16" t="s">
         <v>37</v>
       </c>
@@ -2443,7 +2442,7 @@
         <v>1396</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" s="16" t="s">
         <v>38</v>
       </c>
@@ -2455,7 +2454,7 @@
         <v>11040.5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" s="16" t="s">
         <v>39</v>
       </c>
@@ -2466,7 +2465,7 @@
         <v>2183866</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" s="16" t="s">
         <v>40</v>
       </c>
@@ -2477,7 +2476,7 @@
         <v>2197605</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" s="16" t="s">
         <v>41</v>
       </c>
@@ -2488,7 +2487,7 @@
         <v>12790919</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" s="16" t="s">
         <v>42</v>
       </c>
@@ -2499,7 +2498,7 @@
         <v>974631</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" s="16" t="s">
         <v>43</v>
       </c>
@@ -2510,7 +2509,7 @@
         <v>190772</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" s="16" t="s">
         <v>44</v>
       </c>
@@ -2521,7 +2520,7 @@
         <v>1656</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" s="16" t="s">
         <v>45</v>
       </c>
@@ -2532,7 +2531,7 @@
         <v>1829</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" s="16" t="s">
         <v>46</v>
       </c>
@@ -2543,7 +2542,7 @@
         <v>11464</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" s="16" t="s">
         <v>47</v>
       </c>
@@ -2554,7 +2553,7 @@
         <v>3125</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" s="16" t="s">
         <v>48</v>
       </c>
@@ -2565,7 +2564,7 @@
         <v>679854</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" s="16" t="s">
         <v>49</v>
       </c>
@@ -2576,7 +2575,7 @@
         <v>4441949</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" s="16" t="s">
         <v>50</v>
       </c>
@@ -2587,7 +2586,7 @@
         <v>100562</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" s="16" t="s">
         <v>51</v>
       </c>
@@ -2598,7 +2597,7 @@
         <v>1495511</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" s="16" t="s">
         <v>52</v>
       </c>
@@ -2609,7 +2608,7 @@
         <v>86586</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" s="16" t="s">
         <v>53</v>
       </c>
@@ -2620,7 +2619,7 @@
         <v>1378966</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A29" s="16" t="s">
         <v>54</v>
       </c>
@@ -2631,7 +2630,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30" s="16" t="s">
         <v>55</v>
       </c>
@@ -2642,7 +2641,7 @@
         <v>1084</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31" s="16" t="s">
         <v>56</v>
       </c>
@@ -2653,7 +2652,7 @@
         <v>1086</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32" s="16" t="s">
         <v>57</v>
       </c>
@@ -2664,7 +2663,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A33" s="16" t="s">
         <v>58</v>
       </c>
@@ -2675,7 +2674,7 @@
         <v>8456</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34" s="16" t="s">
         <v>59</v>
       </c>
@@ -2686,7 +2685,7 @@
         <v>4248292</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35" s="16" t="s">
         <v>60</v>
       </c>
@@ -2697,7 +2696,7 @@
         <v>46888</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A36" s="16" t="s">
         <v>61</v>
       </c>
@@ -2708,7 +2707,7 @@
         <v>1287187</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A37" s="16" t="s">
         <v>62</v>
       </c>
@@ -2719,7 +2718,7 @@
         <v>1722207</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A38" s="16" t="s">
         <v>63</v>
       </c>
@@ -2730,7 +2729,7 @@
         <v>2201</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A39" s="16" t="s">
         <v>64</v>
       </c>
@@ -2741,7 +2740,7 @@
         <v>561305</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A40" s="16" t="s">
         <v>65</v>
       </c>
@@ -2752,7 +2751,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A41" s="16" t="s">
         <v>66</v>
       </c>
@@ -2763,7 +2762,7 @@
         <v>43114</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A42" s="16" t="s">
         <v>67</v>
       </c>
@@ -2774,7 +2773,7 @@
         <v>825030</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A43" s="16" t="s">
         <v>68</v>
       </c>
@@ -2785,7 +2784,7 @@
         <v>158926</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A44" s="16" t="s">
         <v>69</v>
       </c>
@@ -2796,7 +2795,7 @@
         <v>366121</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A45" s="16" t="s">
         <v>70</v>
       </c>
@@ -2807,7 +2806,7 @@
         <v>158926</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A46" s="16" t="s">
         <v>71</v>
       </c>
@@ -2818,7 +2817,7 @@
         <v>1548</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A47" s="16" t="s">
         <v>72</v>
       </c>
@@ -2829,7 +2828,7 @@
         <v>74626</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A48" s="16" t="s">
         <v>73</v>
       </c>
@@ -2841,7 +2840,7 @@
         <v>11040.5</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A49" s="16" t="s">
         <v>74</v>
       </c>
@@ -2852,7 +2851,7 @@
         <v>1356</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A50" s="16" t="s">
         <v>75</v>
       </c>
@@ -2863,7 +2862,7 @@
         <v>164587</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A51" s="16" t="s">
         <v>76</v>
       </c>
@@ -2880,20 +2879,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B1" s="11" t="s">
         <v>79</v>
       </c>
@@ -2901,7 +2900,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="16" t="s">
         <v>27</v>
       </c>
@@ -2923,7 +2922,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="16" t="s">
         <v>28</v>
       </c>
@@ -2935,7 +2934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="16" t="s">
         <v>29</v>
       </c>
@@ -2947,7 +2946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="16" t="s">
         <v>30</v>
       </c>
@@ -2959,7 +2958,7 @@
         <v>446750000</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="16" t="s">
         <v>31</v>
       </c>
@@ -2971,7 +2970,7 @@
         <v>487500000</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="16" t="s">
         <v>32</v>
       </c>
@@ -2983,7 +2982,7 @@
         <v>186750000</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="16" t="s">
         <v>33</v>
       </c>
@@ -2995,7 +2994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="16" t="s">
         <v>34</v>
       </c>
@@ -3007,7 +3006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="16" t="s">
         <v>35</v>
       </c>
@@ -3019,7 +3018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="16" t="s">
         <v>36</v>
       </c>
@@ -3031,7 +3030,7 @@
         <v>630875000</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="16" t="s">
         <v>37</v>
       </c>
@@ -3043,7 +3042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="16" t="s">
         <v>38</v>
       </c>
@@ -3055,7 +3054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="16" t="s">
         <v>39</v>
       </c>
@@ -3067,7 +3066,7 @@
         <v>238500000</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="16" t="s">
         <v>40</v>
       </c>
@@ -3079,7 +3078,7 @@
         <v>1256000000</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="16" t="s">
         <v>41</v>
       </c>
@@ -3091,7 +3090,7 @@
         <v>2135500000</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" s="16" t="s">
         <v>42</v>
       </c>
@@ -3103,7 +3102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" s="16" t="s">
         <v>43</v>
       </c>
@@ -3115,7 +3114,7 @@
         <v>184750000</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" s="16" t="s">
         <v>44</v>
       </c>
@@ -3127,7 +3126,7 @@
         <v>65625000</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" s="16" t="s">
         <v>45</v>
       </c>
@@ -3139,7 +3138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" s="16" t="s">
         <v>46</v>
       </c>
@@ -3151,7 +3150,7 @@
         <v>9875000</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" s="16" t="s">
         <v>47</v>
       </c>
@@ -3163,7 +3162,7 @@
         <v>5875000</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" s="16" t="s">
         <v>48</v>
       </c>
@@ -3175,7 +3174,7 @@
         <v>564625000</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" s="16" t="s">
         <v>49</v>
       </c>
@@ -3187,7 +3186,7 @@
         <v>407000000</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" s="16" t="s">
         <v>50</v>
       </c>
@@ -3199,7 +3198,7 @@
         <v>176000000</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" s="16" t="s">
         <v>51</v>
       </c>
@@ -3211,7 +3210,7 @@
         <v>466625000</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" s="16" t="s">
         <v>52</v>
       </c>
@@ -3223,7 +3222,7 @@
         <v>41375000</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" s="16" t="s">
         <v>53</v>
       </c>
@@ -3235,7 +3234,7 @@
         <v>332625000</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A29" s="16" t="s">
         <v>54</v>
       </c>
@@ -3247,7 +3246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30" s="16" t="s">
         <v>55</v>
       </c>
@@ -3259,7 +3258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31" s="16" t="s">
         <v>56</v>
       </c>
@@ -3271,7 +3270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32" s="16" t="s">
         <v>57</v>
       </c>
@@ -3283,7 +3282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A33" s="16" t="s">
         <v>58</v>
       </c>
@@ -3295,7 +3294,7 @@
         <v>209250000</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34" s="16" t="s">
         <v>59</v>
       </c>
@@ -3307,7 +3306,7 @@
         <v>473875000</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35" s="16" t="s">
         <v>60</v>
       </c>
@@ -3319,7 +3318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A36" s="16" t="s">
         <v>61</v>
       </c>
@@ -3331,7 +3330,7 @@
         <v>1338125000</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A37" s="16" t="s">
         <v>62</v>
       </c>
@@ -3343,7 +3342,7 @@
         <v>88250000</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A38" s="16" t="s">
         <v>63</v>
       </c>
@@ -3355,7 +3354,7 @@
         <v>87875000</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A39" s="16" t="s">
         <v>64</v>
       </c>
@@ -3367,7 +3366,7 @@
         <v>1117750000</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A40" s="16" t="s">
         <v>65</v>
       </c>
@@ -3379,7 +3378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A41" s="16" t="s">
         <v>66</v>
       </c>
@@ -3391,7 +3390,7 @@
         <v>133000000</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A42" s="16" t="s">
         <v>67</v>
       </c>
@@ -3403,7 +3402,7 @@
         <v>106750000</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A43" s="16" t="s">
         <v>68</v>
       </c>
@@ -3415,7 +3414,7 @@
         <v>43125000</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A44" s="16" t="s">
         <v>69</v>
       </c>
@@ -3427,7 +3426,7 @@
         <v>757250000</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A45" s="16" t="s">
         <v>70</v>
       </c>
@@ -3439,7 +3438,7 @@
         <v>181250000</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A46" s="16" t="s">
         <v>71</v>
       </c>
@@ -3451,7 +3450,7 @@
         <v>7250000</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A47" s="16" t="s">
         <v>72</v>
       </c>
@@ -3463,7 +3462,7 @@
         <v>92625000</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A48" s="16" t="s">
         <v>73</v>
       </c>
@@ -3475,7 +3474,7 @@
         <v>259875000</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A49" s="16" t="s">
         <v>74</v>
       </c>
@@ -3487,7 +3486,7 @@
         <v>38250000</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A50" s="16" t="s">
         <v>75</v>
       </c>
@@ -3499,7 +3498,7 @@
         <v>270375000</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A51" s="16" t="s">
         <v>76</v>
       </c>
@@ -3517,22 +3516,22 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="39.6640625" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.33203125" customWidth="1"/>
-    <col min="4" max="5" width="12.83203125" customWidth="1"/>
+    <col min="4" max="5" width="12.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
@@ -3550,7 +3549,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
         <v>10</v>
       </c>
@@ -3563,15 +3562,15 @@
       </c>
       <c r="D2" s="6">
         <f>INDEX('Egg production'!C:C,MATCH(About!B1,'Egg production'!A:A,0))</f>
-        <v>407000000</v>
+        <v>87875000</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="10">
         <f>SUMPRODUCT(C2:C6,D2:D6)/SUM(D2:D6)</f>
-        <v>7.7196438360556785</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>7.9801120990445451</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
         <v>18</v>
       </c>
@@ -3584,12 +3583,12 @@
       </c>
       <c r="D3" s="9">
         <f>INDEX('Broiler production'!C:C,MATCH(About!B1,'Broiler production'!A:A,0))</f>
-        <v>222935131.05131638</v>
+        <v>0</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>11</v>
       </c>
@@ -3602,12 +3601,12 @@
       </c>
       <c r="D4" s="14">
         <f>INDEX('Dairy production'!B:B,MATCH(About!B1,'Dairy production'!A:A,0))</f>
-        <v>8255844823</v>
+        <v>2394966049</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
         <v>12</v>
       </c>
@@ -3620,12 +3619,12 @@
       </c>
       <c r="D5" s="9">
         <f>INDEX('Beef and pork production'!C:C,MATCH(About!B1,'Beef and pork production'!A:A,0))*1000</f>
-        <v>4441949000</v>
+        <v>2201000</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="6" t="s">
         <v>13</v>
       </c>
@@ -3638,7 +3637,7 @@
       </c>
       <c r="D6" s="9">
         <f>INDEX('Beef and pork production'!B:B,MATCH(About!B1,'Beef and pork production'!A:A,0))*1000</f>
-        <v>1407277000</v>
+        <v>592400000</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="6"/>
@@ -3650,7 +3649,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
@@ -3660,23 +3659,23 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="40" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A2" s="11" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="4">
         <f>Calculations!F2</f>
-        <v>7.7196438360556785</v>
+        <v>7.9801120990445451</v>
       </c>
     </row>
   </sheetData>

</xml_diff>